<commit_message>
Updated descriptions on BOM
</commit_message>
<xml_diff>
--- a/mechanical/Test Engine BOM.xlsx
+++ b/mechanical/Test Engine BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Item</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>Acquired</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>O-ring</t>
+  </si>
+  <si>
+    <t>M10 x1</t>
   </si>
 </sst>
 </file>
@@ -468,13 +477,13 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -508,6 +517,9 @@
       <c r="C3" s="1">
         <v>4</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
@@ -516,6 +528,9 @@
       <c r="C4" s="1">
         <v>4</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
@@ -569,6 +584,9 @@
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C11" s="1">
         <v>2</v>
       </c>
@@ -640,6 +658,9 @@
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>

</xml_diff>